<commit_message>
[FIX] #2663 debug error and format excel
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_invest_construction_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_invest_construction_report.xlsx
@@ -303,8 +303,8 @@
   </sheetPr>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q8" activeCellId="0" sqref="Q8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>